<commit_message>
Update test data for removed variables and rely more on moorings & installation examples
</commit_message>
<xml_diff>
--- a/test_data/operations/electrical_parts.xlsx
+++ b/test_data/operations/electrical_parts.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\test_data\operations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="9000"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="22980" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="On-Site" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Sub-System</t>
   </si>
@@ -40,12 +45,15 @@
   </si>
   <si>
     <t>Export Cable</t>
+  </si>
+  <si>
+    <t>Umbilical Cable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +135,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,7 +146,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -153,6 +160,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -201,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,7 +246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,19 +458,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,8 +487,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1">
@@ -494,8 +504,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1">
@@ -511,8 +521,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1">
@@ -528,12 +538,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -548,16 +568,16 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -585,7 +605,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>